<commit_message>
new way of scraping by search
</commit_message>
<xml_diff>
--- a/testWorksheet.xlsx
+++ b/testWorksheet.xlsx
@@ -393,7 +393,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -403,22 +403,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>30403.97</v>
+        <v>30310.06</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3735.36</v>
+        <v>3727.37</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>12838.86</v>
+        <v>12858.38</v>
       </c>
     </row>
     <row r="4" ht="128.25" customHeight="1">
       <c r="A4" t="n">
-        <v>1996.25</v>
+        <v>1956.37</v>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
@@ -426,6 +426,66 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2705.32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>72.95</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>401.61</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>27568.15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>3379.04</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>119231.84</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1252.33</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>85.23999999999999</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1.67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>